<commit_message>
Update Items, Add Abilities & Moves from Scarlet-Violet
</commit_message>
<xml_diff>
--- a/Crystal PokeDex/Data/Sword&Shield/特性/特性_简中.xlsx
+++ b/Crystal PokeDex/Data/Sword&Shield/特性/特性_简中.xlsx
@@ -362,7 +362,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -375,6 +375,14 @@
       <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="新細明體"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -395,13 +403,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -708,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
+      <selection activeCell="A28" sqref="A28:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -996,7 +1012,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>250</v>
       </c>
@@ -1013,7 +1029,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>251</v>
       </c>
@@ -1030,7 +1046,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>252</v>
       </c>
@@ -1047,7 +1063,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>253</v>
       </c>
@@ -1064,7 +1080,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>254</v>
       </c>
@@ -1081,7 +1097,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>255</v>
       </c>
@@ -1098,7 +1114,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>256</v>
       </c>
@@ -1115,7 +1131,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>257</v>
       </c>
@@ -1132,7 +1148,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>258</v>
       </c>
@@ -1149,7 +1165,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>259</v>
       </c>
@@ -1166,7 +1182,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>260</v>
       </c>
@@ -1182,6 +1198,69 @@
       <c r="E27" t="s">
         <v>106</v>
       </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>